<commit_message>
improved speed of excel data addition
</commit_message>
<xml_diff>
--- a/t_Batch.xlsx
+++ b/t_Batch.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://morningstaronline-my.sharepoint.com/personal/spencer_klug_pitchbook_com/Documents/India_PF_Expansion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_2161480A4276A4DEEC4C5CD4475DCE3A874A08A9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D9330A7-50C3-420A-849D-477A120FE307}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_216194320643A6DFEC4C5CD4475DCE3A874A08A9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36203BAF-6493-47F5-8B6B-971DD27FD90E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AQ$501</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="945">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -2864,11 +2865,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2880,6 +2883,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2914,18 +2924,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3226,16 +3240,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -3426,7 +3477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2503</v>
       </c>
@@ -3470,7 +3521,7 @@
         <v>19658</v>
       </c>
     </row>
-    <row r="6" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2504</v>
       </c>
@@ -3614,7 +3665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2510</v>
       </c>
@@ -3664,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2511</v>
       </c>
@@ -3740,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2513</v>
       </c>
@@ -3804,7 +3855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2515</v>
       </c>
@@ -3935,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2516</v>
       </c>
@@ -4066,7 +4117,7 @@
         <v>1152721</v>
       </c>
     </row>
-    <row r="19" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2517</v>
       </c>
@@ -4277,7 +4328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2522</v>
       </c>
@@ -4333,7 +4384,7 @@
         <v>1957354</v>
       </c>
     </row>
-    <row r="25" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2523</v>
       </c>
@@ -4389,7 +4440,7 @@
         <v>126339</v>
       </c>
     </row>
-    <row r="26" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2524</v>
       </c>
@@ -4528,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2529</v>
       </c>
@@ -4592,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2531</v>
       </c>
@@ -4756,7 +4807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2538</v>
       </c>
@@ -4815,7 +4866,7 @@
         <v>87150625</v>
       </c>
     </row>
-    <row r="41" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2539</v>
       </c>
@@ -4894,7 +4945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2541</v>
       </c>
@@ -4938,7 +4989,7 @@
         <v>-27794630</v>
       </c>
     </row>
-    <row r="44" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2542</v>
       </c>
@@ -4982,7 +5033,7 @@
         <v>14990367</v>
       </c>
     </row>
-    <row r="45" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2543</v>
       </c>
@@ -5110,7 +5161,7 @@
         <v>6114283</v>
       </c>
     </row>
-    <row r="46" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2544</v>
       </c>
@@ -5241,7 +5292,7 @@
         <v>13485241</v>
       </c>
     </row>
-    <row r="47" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2545</v>
       </c>
@@ -5372,7 +5423,7 @@
         <v>13977126</v>
       </c>
     </row>
-    <row r="48" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2546</v>
       </c>
@@ -5503,7 +5554,7 @@
         <v>11501273</v>
       </c>
     </row>
-    <row r="49" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2547</v>
       </c>
@@ -5634,7 +5685,7 @@
         <v>4224841</v>
       </c>
     </row>
-    <row r="50" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2548</v>
       </c>
@@ -5765,7 +5816,7 @@
         <v>8038815</v>
       </c>
     </row>
-    <row r="51" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2549</v>
       </c>
@@ -5866,7 +5917,7 @@
         <v>3391833</v>
       </c>
     </row>
-    <row r="52" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2550</v>
       </c>
@@ -5967,7 +6018,7 @@
         <v>556896</v>
       </c>
     </row>
-    <row r="53" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>2551</v>
       </c>
@@ -6068,7 +6119,7 @@
         <v>87331</v>
       </c>
     </row>
-    <row r="54" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2552</v>
       </c>
@@ -6127,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2553</v>
       </c>
@@ -6186,7 +6237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2554</v>
       </c>
@@ -6230,7 +6281,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="57" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2555</v>
       </c>
@@ -6334,7 +6385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2559</v>
       </c>
@@ -6462,7 +6513,7 @@
         <v>5111727</v>
       </c>
     </row>
-    <row r="62" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2560</v>
       </c>
@@ -6590,7 +6641,7 @@
         <v>5111727</v>
       </c>
     </row>
-    <row r="63" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2561</v>
       </c>
@@ -6721,7 +6772,7 @@
         <v>652115</v>
       </c>
     </row>
-    <row r="64" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2562</v>
       </c>
@@ -6872,7 +6923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2564</v>
       </c>
@@ -6973,7 +7024,7 @@
         <v>12048236</v>
       </c>
     </row>
-    <row r="67" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2565</v>
       </c>
@@ -7032,7 +7083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2566</v>
       </c>
@@ -7082,7 +7133,7 @@
         <v>39081739</v>
       </c>
     </row>
-    <row r="69" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2567</v>
       </c>
@@ -7141,7 +7192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2568</v>
       </c>
@@ -7242,7 +7293,7 @@
         <v>6406128</v>
       </c>
     </row>
-    <row r="71" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2569</v>
       </c>
@@ -7343,7 +7394,7 @@
         <v>3440282</v>
       </c>
     </row>
-    <row r="72" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2570</v>
       </c>
@@ -7396,7 +7447,7 @@
         <v>9430436</v>
       </c>
     </row>
-    <row r="73" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2571</v>
       </c>
@@ -7460,7 +7511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>2573</v>
       </c>
@@ -7504,7 +7555,7 @@
         <v>679149</v>
       </c>
     </row>
-    <row r="76" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2574</v>
       </c>
@@ -7557,7 +7608,7 @@
         <v>10606391</v>
       </c>
     </row>
-    <row r="77" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2575</v>
       </c>
@@ -7610,7 +7661,7 @@
         <v>16019153</v>
       </c>
     </row>
-    <row r="78" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2576</v>
       </c>
@@ -7738,7 +7789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>2577</v>
       </c>
@@ -7866,7 +7917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2578</v>
       </c>
@@ -8034,7 +8085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>2581</v>
       </c>
@@ -8165,7 +8216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>2582</v>
       </c>
@@ -8293,7 +8344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>2583</v>
       </c>
@@ -8424,7 +8475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>2584</v>
       </c>
@@ -8615,7 +8666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>2588</v>
       </c>
@@ -8746,7 +8797,7 @@
         <v>27287270</v>
       </c>
     </row>
-    <row r="91" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>2589</v>
       </c>
@@ -8877,7 +8928,7 @@
         <v>795730</v>
       </c>
     </row>
-    <row r="92" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>2590</v>
       </c>
@@ -9005,7 +9056,7 @@
         <v>852949</v>
       </c>
     </row>
-    <row r="93" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>2591</v>
       </c>
@@ -9106,7 +9157,7 @@
         <v>436493</v>
       </c>
     </row>
-    <row r="94" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>2592</v>
       </c>
@@ -9207,7 +9258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>2593</v>
       </c>
@@ -9308,7 +9359,7 @@
         <v>804052</v>
       </c>
     </row>
-    <row r="96" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>2594</v>
       </c>
@@ -9439,7 +9490,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="97" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>2595</v>
       </c>
@@ -9570,7 +9621,7 @@
         <v>1156345</v>
       </c>
     </row>
-    <row r="98" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>2596</v>
       </c>
@@ -9701,7 +9752,7 @@
         <v>17384</v>
       </c>
     </row>
-    <row r="99" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>2597</v>
       </c>
@@ -9832,7 +9883,7 @@
         <v>21151</v>
       </c>
     </row>
-    <row r="100" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>2598</v>
       </c>
@@ -10103,7 +10154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>2606</v>
       </c>
@@ -10162,7 +10213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2607</v>
       </c>
@@ -10283,7 +10334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>2609</v>
       </c>
@@ -10414,7 +10465,7 @@
         <v>1730079</v>
       </c>
     </row>
-    <row r="112" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>2610</v>
       </c>
@@ -10545,7 +10596,7 @@
         <v>454944</v>
       </c>
     </row>
-    <row r="113" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>2611</v>
       </c>
@@ -10676,7 +10727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>2612</v>
       </c>
@@ -10807,7 +10858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>2613</v>
       </c>
@@ -10851,7 +10902,7 @@
         <v>6545</v>
       </c>
     </row>
-    <row r="116" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>2614</v>
       </c>
@@ -10898,7 +10949,7 @@
         <v>5745</v>
       </c>
     </row>
-    <row r="117" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>2615</v>
       </c>
@@ -10993,7 +11044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>2619</v>
       </c>
@@ -11124,7 +11175,7 @@
         <v>8871</v>
       </c>
     </row>
-    <row r="122" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>2620</v>
       </c>
@@ -11255,7 +11306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2621</v>
       </c>
@@ -11383,7 +11434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>2622</v>
       </c>
@@ -11484,7 +11535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>2623</v>
       </c>
@@ -11543,7 +11594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>2624</v>
       </c>
@@ -11602,7 +11653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>2625</v>
       </c>
@@ -11661,7 +11712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>2626</v>
       </c>
@@ -11762,7 +11813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>2627</v>
       </c>
@@ -11818,7 +11869,7 @@
         <v>13796806</v>
       </c>
     </row>
-    <row r="130" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>2628</v>
       </c>
@@ -11919,7 +11970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2629</v>
       </c>
@@ -11972,7 +12023,7 @@
         <v>181441</v>
       </c>
     </row>
-    <row r="132" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2630</v>
       </c>
@@ -12016,7 +12067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>2631</v>
       </c>
@@ -12060,7 +12111,7 @@
         <v>3148</v>
       </c>
     </row>
-    <row r="134" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>2632</v>
       </c>
@@ -12104,7 +12155,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="135" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>2633</v>
       </c>
@@ -12157,7 +12208,7 @@
         <v>-731227</v>
       </c>
     </row>
-    <row r="136" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>2634</v>
       </c>
@@ -12201,7 +12252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>2635</v>
       </c>
@@ -12354,7 +12405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>2641</v>
       </c>
@@ -12482,7 +12533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>2642</v>
       </c>
@@ -12532,7 +12583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>2643</v>
       </c>
@@ -12633,7 +12684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>2644</v>
       </c>
@@ -12734,7 +12785,7 @@
         <v>4235635</v>
       </c>
     </row>
-    <row r="147" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2645</v>
       </c>
@@ -12793,7 +12844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>2646</v>
       </c>
@@ -12894,7 +12945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>2647</v>
       </c>
@@ -13024,7 +13075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>2652</v>
       </c>
@@ -13152,7 +13203,7 @@
         <v>2418677</v>
       </c>
     </row>
-    <row r="155" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>2653</v>
       </c>
@@ -13353,7 +13404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>2659</v>
       </c>
@@ -13406,7 +13457,7 @@
         <v>3500488</v>
       </c>
     </row>
-    <row r="162" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>2660</v>
       </c>
@@ -13459,7 +13510,7 @@
         <v>3395760</v>
       </c>
     </row>
-    <row r="163" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>2661</v>
       </c>
@@ -13518,7 +13569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>2662</v>
       </c>
@@ -13651,7 +13702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>2667</v>
       </c>
@@ -13695,7 +13746,7 @@
         <v>3596</v>
       </c>
     </row>
-    <row r="170" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>2668</v>
       </c>
@@ -13739,7 +13790,7 @@
         <v>3962</v>
       </c>
     </row>
-    <row r="171" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>2669</v>
       </c>
@@ -13783,7 +13834,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="172" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>2670</v>
       </c>
@@ -13967,7 +14018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>2678</v>
       </c>
@@ -14017,7 +14068,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="181" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>2679</v>
       </c>
@@ -14116,7 +14167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>2682</v>
       </c>
@@ -14160,7 +14211,7 @@
         <v>2805547</v>
       </c>
     </row>
-    <row r="185" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>2683</v>
       </c>
@@ -14291,7 +14342,7 @@
         <v>132100000</v>
       </c>
     </row>
-    <row r="186" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>2684</v>
       </c>
@@ -14422,7 +14473,7 @@
         <v>132100000</v>
       </c>
     </row>
-    <row r="187" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>2685</v>
       </c>
@@ -14553,7 +14604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>2686</v>
       </c>
@@ -14684,7 +14735,7 @@
         <v>132100000</v>
       </c>
     </row>
-    <row r="189" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>2687</v>
       </c>
@@ -14815,7 +14866,7 @@
         <v>308657065</v>
       </c>
     </row>
-    <row r="190" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>2688</v>
       </c>
@@ -14946,7 +14997,7 @@
         <v>479239767</v>
       </c>
     </row>
-    <row r="191" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>2689</v>
       </c>
@@ -15074,7 +15125,7 @@
         <v>211705535</v>
       </c>
     </row>
-    <row r="192" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>2690</v>
       </c>
@@ -15205,7 +15256,7 @@
         <v>179879869</v>
       </c>
     </row>
-    <row r="193" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>2691</v>
       </c>
@@ -15336,7 +15387,7 @@
         <v>194405874</v>
       </c>
     </row>
-    <row r="194" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>2692</v>
       </c>
@@ -15467,7 +15518,7 @@
         <v>525805399</v>
       </c>
     </row>
-    <row r="195" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>2693</v>
       </c>
@@ -15523,7 +15574,7 @@
         <v>161539082</v>
       </c>
     </row>
-    <row r="196" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>2694</v>
       </c>
@@ -15624,7 +15675,7 @@
         <v>91755616</v>
       </c>
     </row>
-    <row r="197" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>2695</v>
       </c>
@@ -15683,7 +15734,7 @@
         <v>2936267</v>
       </c>
     </row>
-    <row r="198" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>2696</v>
       </c>
@@ -15784,7 +15835,7 @@
         <v>136527564</v>
       </c>
     </row>
-    <row r="199" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>2697</v>
       </c>
@@ -15843,7 +15894,7 @@
         <v>4730264</v>
       </c>
     </row>
-    <row r="200" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>2698</v>
       </c>
@@ -15944,7 +15995,7 @@
         <v>102763709</v>
       </c>
     </row>
-    <row r="201" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>2699</v>
       </c>
@@ -15997,7 +16048,7 @@
         <v>3531868</v>
       </c>
     </row>
-    <row r="202" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>2700</v>
       </c>
@@ -16041,7 +16092,7 @@
         <v>1287357</v>
       </c>
     </row>
-    <row r="203" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>2701</v>
       </c>
@@ -16094,7 +16145,7 @@
         <v>12024079</v>
       </c>
     </row>
-    <row r="204" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>2702</v>
       </c>
@@ -16138,7 +16189,7 @@
         <v>1568495</v>
       </c>
     </row>
-    <row r="205" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>2703</v>
       </c>
@@ -16391,7 +16442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>2714</v>
       </c>
@@ -16426,7 +16477,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="217" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>2715</v>
       </c>
@@ -16565,7 +16616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>2720</v>
       </c>
@@ -16693,7 +16744,7 @@
         <v>6996986</v>
       </c>
     </row>
-    <row r="223" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>2721</v>
       </c>
@@ -16824,7 +16875,7 @@
         <v>6885237</v>
       </c>
     </row>
-    <row r="224" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>2722</v>
       </c>
@@ -16925,7 +16976,7 @@
         <v>2430934</v>
       </c>
     </row>
-    <row r="225" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>2723</v>
       </c>
@@ -16984,7 +17035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>2724</v>
       </c>
@@ -17034,7 +17085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>2725</v>
       </c>
@@ -17084,7 +17135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>2726</v>
       </c>
@@ -17185,7 +17236,7 @@
         <v>7467480</v>
       </c>
     </row>
-    <row r="229" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>2727</v>
       </c>
@@ -17286,7 +17337,7 @@
         <v>7943754</v>
       </c>
     </row>
-    <row r="230" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>2728</v>
       </c>
@@ -17417,7 +17468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>2729</v>
       </c>
@@ -17548,7 +17599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>2730</v>
       </c>
@@ -17679,7 +17730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>2731</v>
       </c>
@@ -17890,7 +17941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>2736</v>
       </c>
@@ -18029,7 +18080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>2741</v>
       </c>
@@ -18213,7 +18264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>2749</v>
       </c>
@@ -18272,7 +18323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>2750</v>
       </c>
@@ -18351,7 +18402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>2752</v>
       </c>
@@ -18395,7 +18446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>2753</v>
       </c>
@@ -18519,7 +18570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>2758</v>
       </c>
@@ -18647,7 +18698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>2759</v>
       </c>
@@ -18778,7 +18829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>2760</v>
       </c>
@@ -18909,7 +18960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>2761</v>
       </c>
@@ -19010,7 +19061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>2762</v>
       </c>
@@ -19251,7 +19302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>2770</v>
       </c>
@@ -19352,7 +19403,7 @@
         <v>4573300</v>
       </c>
     </row>
-    <row r="273" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>2771</v>
       </c>
@@ -19405,7 +19456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>2772</v>
       </c>
@@ -19506,7 +19557,7 @@
         <v>9512589</v>
       </c>
     </row>
-    <row r="275" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>2773</v>
       </c>
@@ -19559,7 +19610,7 @@
         <v>-35183762</v>
       </c>
     </row>
-    <row r="276" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>2774</v>
       </c>
@@ -19597,7 +19648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>2775</v>
       </c>
@@ -19790,7 +19841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>2783</v>
       </c>
@@ -19891,7 +19942,7 @@
         <v>4162974</v>
       </c>
     </row>
-    <row r="286" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>2784</v>
       </c>
@@ -19944,7 +19995,7 @@
         <v>-842147</v>
       </c>
     </row>
-    <row r="287" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>2785</v>
       </c>
@@ -20023,7 +20074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>2787</v>
       </c>
@@ -20154,7 +20205,7 @@
         <v>141991</v>
       </c>
     </row>
-    <row r="290" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>2788</v>
       </c>
@@ -20282,7 +20333,7 @@
         <v>143840</v>
       </c>
     </row>
-    <row r="291" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>2789</v>
       </c>
@@ -20413,7 +20464,7 @@
         <v>141991</v>
       </c>
     </row>
-    <row r="292" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>2790</v>
       </c>
@@ -20544,7 +20595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>2791</v>
       </c>
@@ -20675,7 +20726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>2792</v>
       </c>
@@ -20734,7 +20785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>2793</v>
       </c>
@@ -20784,7 +20835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>2794</v>
       </c>
@@ -20885,7 +20936,7 @@
         <v>785174</v>
       </c>
     </row>
-    <row r="297" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>2795</v>
       </c>
@@ -20986,7 +21037,7 @@
         <v>777116</v>
       </c>
     </row>
-    <row r="298" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>2796</v>
       </c>
@@ -21087,7 +21138,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="299" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>2797</v>
       </c>
@@ -21206,7 +21257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>2801</v>
       </c>
@@ -21337,7 +21388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>2802</v>
       </c>
@@ -21396,7 +21447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>2803</v>
       </c>
@@ -21443,7 +21494,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="306" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>2804</v>
       </c>
@@ -21490,7 +21541,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="307" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>2805</v>
       </c>
@@ -21621,7 +21672,7 @@
         <v>2791629</v>
       </c>
     </row>
-    <row r="308" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>2806</v>
       </c>
@@ -21749,7 +21800,7 @@
         <v>4281762</v>
       </c>
     </row>
-    <row r="309" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>2807</v>
       </c>
@@ -21880,7 +21931,7 @@
         <v>2865667</v>
       </c>
     </row>
-    <row r="310" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>2808</v>
       </c>
@@ -22011,7 +22062,7 @@
         <v>3087981</v>
       </c>
     </row>
-    <row r="311" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>2809</v>
       </c>
@@ -22142,7 +22193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>2810</v>
       </c>
@@ -22273,7 +22324,7 @@
         <v>3451523</v>
       </c>
     </row>
-    <row r="313" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>2811</v>
       </c>
@@ -22332,7 +22383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>2812</v>
       </c>
@@ -22433,7 +22484,7 @@
         <v>35600</v>
       </c>
     </row>
-    <row r="315" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>2813</v>
       </c>
@@ -22483,7 +22534,7 @@
         <v>4275</v>
       </c>
     </row>
-    <row r="316" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>2814</v>
       </c>
@@ -22584,7 +22635,7 @@
         <v>796806</v>
       </c>
     </row>
-    <row r="317" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>2815</v>
       </c>
@@ -22685,7 +22736,7 @@
         <v>2894163</v>
       </c>
     </row>
-    <row r="318" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>2816</v>
       </c>
@@ -22824,7 +22875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>2821</v>
       </c>
@@ -22883,7 +22934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>2822</v>
       </c>
@@ -22942,7 +22993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>2823</v>
       </c>
@@ -23001,7 +23052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>2824</v>
       </c>
@@ -23048,7 +23099,7 @@
         <v>6571042</v>
       </c>
     </row>
-    <row r="327" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>2825</v>
       </c>
@@ -23092,7 +23143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>2826</v>
       </c>
@@ -23136,7 +23187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>2827</v>
       </c>
@@ -23177,7 +23228,7 @@
         <v>7361033</v>
       </c>
     </row>
-    <row r="330" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>2828</v>
       </c>
@@ -23341,7 +23392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>2835</v>
       </c>
@@ -23400,7 +23451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>2836</v>
       </c>
@@ -23459,7 +23510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>2837</v>
       </c>
@@ -23538,7 +23589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>2839</v>
       </c>
@@ -23642,7 +23693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>2843</v>
       </c>
@@ -23773,7 +23824,7 @@
         <v>2081494</v>
       </c>
     </row>
-    <row r="346" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>2844</v>
       </c>
@@ -23904,7 +23955,7 @@
         <v>123232</v>
       </c>
     </row>
-    <row r="347" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>2845</v>
       </c>
@@ -23963,7 +24014,7 @@
         <v>491033</v>
       </c>
     </row>
-    <row r="348" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>2846</v>
       </c>
@@ -24001,7 +24052,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="349" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>2847</v>
       </c>
@@ -24042,7 +24093,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="350" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>2848</v>
       </c>
@@ -24086,7 +24137,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="351" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>2849</v>
       </c>
@@ -24217,7 +24268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>2850</v>
       </c>
@@ -24345,7 +24396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>2851</v>
       </c>
@@ -24476,7 +24527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>2852</v>
       </c>
@@ -24607,7 +24658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>2853</v>
       </c>
@@ -24738,7 +24789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>2854</v>
       </c>
@@ -24839,7 +24890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>2855</v>
       </c>
@@ -24889,7 +24940,7 @@
         <v>549976</v>
       </c>
     </row>
-    <row r="358" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>2856</v>
       </c>
@@ -24990,7 +25041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>2857</v>
       </c>
@@ -25040,7 +25091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>2858</v>
       </c>
@@ -25141,7 +25192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>2859</v>
       </c>
@@ -25191,7 +25242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>2860</v>
       </c>
@@ -25241,7 +25292,7 @@
         <v>31648</v>
       </c>
     </row>
-    <row r="363" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>2861</v>
       </c>
@@ -25291,7 +25342,7 @@
         <v>36711</v>
       </c>
     </row>
-    <row r="364" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>2862</v>
       </c>
@@ -25422,7 +25473,7 @@
         <v>1333450</v>
       </c>
     </row>
-    <row r="365" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>2863</v>
       </c>
@@ -25553,7 +25604,7 @@
         <v>2852160</v>
       </c>
     </row>
-    <row r="366" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>2864</v>
       </c>
@@ -25684,7 +25735,7 @@
         <v>545599</v>
       </c>
     </row>
-    <row r="367" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>2865</v>
       </c>
@@ -25815,7 +25866,7 @@
         <v>1006260</v>
       </c>
     </row>
-    <row r="368" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>2866</v>
       </c>
@@ -25943,7 +25994,7 @@
         <v>252906</v>
       </c>
     </row>
-    <row r="369" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>2867</v>
       </c>
@@ -26074,7 +26125,7 @@
         <v>1273977</v>
       </c>
     </row>
-    <row r="370" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>2868</v>
       </c>
@@ -26175,7 +26226,7 @@
         <v>1606872</v>
       </c>
     </row>
-    <row r="371" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>2869</v>
       </c>
@@ -26276,7 +26327,7 @@
         <v>340452</v>
       </c>
     </row>
-    <row r="372" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>2870</v>
       </c>
@@ -26326,7 +26377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>2871</v>
       </c>
@@ -26385,7 +26436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>2872</v>
       </c>
@@ -26486,7 +26537,7 @@
         <v>578937</v>
       </c>
     </row>
-    <row r="375" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>2873</v>
       </c>
@@ -26625,7 +26676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>2878</v>
       </c>
@@ -26681,7 +26732,7 @@
         <v>109985060</v>
       </c>
     </row>
-    <row r="381" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>2879</v>
       </c>
@@ -26737,7 +26788,7 @@
         <v>96316</v>
       </c>
     </row>
-    <row r="382" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>2880</v>
       </c>
@@ -26876,7 +26927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>2885</v>
       </c>
@@ -26935,7 +26986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>2886</v>
       </c>
@@ -27065,7 +27116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>2891</v>
       </c>
@@ -27196,7 +27247,7 @@
         <v>4130338</v>
       </c>
     </row>
-    <row r="394" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>2892</v>
       </c>
@@ -27327,7 +27378,7 @@
         <v>3873911</v>
       </c>
     </row>
-    <row r="395" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>2893</v>
       </c>
@@ -27458,7 +27509,7 @@
         <v>8480052</v>
       </c>
     </row>
-    <row r="396" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>2894</v>
       </c>
@@ -27589,7 +27640,7 @@
         <v>5499955</v>
       </c>
     </row>
-    <row r="397" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>2895</v>
       </c>
@@ -27717,7 +27768,7 @@
         <v>741902</v>
       </c>
     </row>
-    <row r="398" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>2896</v>
       </c>
@@ -27848,7 +27899,7 @@
         <v>5147252</v>
       </c>
     </row>
-    <row r="399" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>2897</v>
       </c>
@@ -27949,7 +28000,7 @@
         <v>603107</v>
       </c>
     </row>
-    <row r="400" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>2898</v>
       </c>
@@ -28110,7 +28161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>2902</v>
       </c>
@@ -28241,7 +28292,7 @@
         <v>53481914</v>
       </c>
     </row>
-    <row r="405" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>2903</v>
       </c>
@@ -28372,7 +28423,7 @@
         <v>80388130</v>
       </c>
     </row>
-    <row r="406" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>2904</v>
       </c>
@@ -28503,7 +28554,7 @@
         <v>29619957</v>
       </c>
     </row>
-    <row r="407" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>2905</v>
       </c>
@@ -28604,7 +28655,7 @@
         <v>3646922</v>
       </c>
     </row>
-    <row r="408" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>2906</v>
       </c>
@@ -28705,7 +28756,7 @@
         <v>9037998</v>
       </c>
     </row>
-    <row r="409" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>2907</v>
       </c>
@@ -28806,7 +28857,7 @@
         <v>9037998</v>
       </c>
     </row>
-    <row r="410" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>2908</v>
       </c>
@@ -28907,7 +28958,7 @@
         <v>7364222</v>
       </c>
     </row>
-    <row r="411" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>2909</v>
       </c>
@@ -29017,7 +29068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>2913</v>
       </c>
@@ -29055,7 +29106,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="416" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>2914</v>
       </c>
@@ -29096,7 +29147,7 @@
         <v>36243</v>
       </c>
     </row>
-    <row r="417" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>2915</v>
       </c>
@@ -29152,7 +29203,7 @@
         <v>49643198</v>
       </c>
     </row>
-    <row r="418" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>2916</v>
       </c>
@@ -29283,7 +29334,7 @@
         <v>426336</v>
       </c>
     </row>
-    <row r="419" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>2917</v>
       </c>
@@ -29414,7 +29465,7 @@
         <v>412789</v>
       </c>
     </row>
-    <row r="420" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>2918</v>
       </c>
@@ -29545,7 +29596,7 @@
         <v>2977378</v>
       </c>
     </row>
-    <row r="421" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>2919</v>
       </c>
@@ -29676,7 +29727,7 @@
         <v>522823</v>
       </c>
     </row>
-    <row r="422" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>2920</v>
       </c>
@@ -29807,7 +29858,7 @@
         <v>825446</v>
       </c>
     </row>
-    <row r="423" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>2921</v>
       </c>
@@ -29938,7 +29989,7 @@
         <v>6483949</v>
       </c>
     </row>
-    <row r="424" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>2922</v>
       </c>
@@ -30039,7 +30090,7 @@
         <v>1283132</v>
       </c>
     </row>
-    <row r="425" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>2923</v>
       </c>
@@ -30095,7 +30146,7 @@
         <v>51016342</v>
       </c>
     </row>
-    <row r="426" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>2924</v>
       </c>
@@ -30148,7 +30199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <v>2925</v>
       </c>
@@ -30249,7 +30300,7 @@
         <v>20335</v>
       </c>
     </row>
-    <row r="428" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <v>2926</v>
       </c>
@@ -30468,7 +30519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>2935</v>
       </c>
@@ -30596,7 +30647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>2936</v>
       </c>
@@ -30727,7 +30778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>2937</v>
       </c>
@@ -30828,7 +30879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <v>2938</v>
       </c>
@@ -30887,7 +30938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>2939</v>
       </c>
@@ -30946,7 +30997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>2940</v>
       </c>
@@ -31005,7 +31056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
         <v>2941</v>
       </c>
@@ -31064,7 +31115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A444" s="1">
         <v>2942</v>
       </c>
@@ -31123,7 +31174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
         <v>2943</v>
       </c>
@@ -31182,7 +31233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <v>2944</v>
       </c>
@@ -31283,7 +31334,7 @@
         <v>6540</v>
       </c>
     </row>
-    <row r="447" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
         <v>2945</v>
       </c>
@@ -31384,7 +31435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A448" s="1">
         <v>2946</v>
       </c>
@@ -31443,7 +31494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
         <v>2947</v>
       </c>
@@ -31502,7 +31553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <v>2948</v>
       </c>
@@ -31546,7 +31597,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="451" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
         <v>2949</v>
       </c>
@@ -31590,7 +31641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
         <v>2950</v>
       </c>
@@ -31721,7 +31772,7 @@
         <v>13375713</v>
       </c>
     </row>
-    <row r="453" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <v>2951</v>
       </c>
@@ -31852,7 +31903,7 @@
         <v>13375713</v>
       </c>
     </row>
-    <row r="454" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
         <v>2952</v>
       </c>
@@ -31983,7 +32034,7 @@
         <v>38250045</v>
       </c>
     </row>
-    <row r="455" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
         <v>2953</v>
       </c>
@@ -32114,7 +32165,7 @@
         <v>45151783</v>
       </c>
     </row>
-    <row r="456" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
         <v>2954</v>
       </c>
@@ -32245,7 +32296,7 @@
         <v>8524000</v>
       </c>
     </row>
-    <row r="457" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
         <v>2955</v>
       </c>
@@ -32373,7 +32424,7 @@
         <v>555000</v>
       </c>
     </row>
-    <row r="458" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
         <v>2956</v>
       </c>
@@ -32501,7 +32552,7 @@
         <v>555000</v>
       </c>
     </row>
-    <row r="459" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
         <v>2957</v>
       </c>
@@ -32632,7 +32683,7 @@
         <v>29183637</v>
       </c>
     </row>
-    <row r="460" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <v>2958</v>
       </c>
@@ -32733,7 +32784,7 @@
         <v>1181750</v>
       </c>
     </row>
-    <row r="461" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
         <v>2959</v>
       </c>
@@ -32834,7 +32885,7 @@
         <v>649650</v>
       </c>
     </row>
-    <row r="462" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
         <v>2960</v>
       </c>
@@ -32935,7 +32986,7 @@
         <v>550550</v>
       </c>
     </row>
-    <row r="463" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
         <v>2961</v>
       </c>
@@ -32994,7 +33045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A464" s="1">
         <v>2962</v>
       </c>
@@ -33053,7 +33104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
         <v>2963</v>
       </c>
@@ -33112,7 +33163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
         <v>2964</v>
       </c>
@@ -33162,7 +33213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
         <v>2965</v>
       </c>
@@ -33215,7 +33266,7 @@
         <v>7739</v>
       </c>
     </row>
-    <row r="468" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
         <v>2966</v>
       </c>
@@ -33268,7 +33319,7 @@
         <v>73514</v>
       </c>
     </row>
-    <row r="469" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A469" s="1">
         <v>2967</v>
       </c>
@@ -33321,7 +33372,7 @@
         <v>-24446</v>
       </c>
     </row>
-    <row r="470" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
         <v>2968</v>
       </c>
@@ -33365,7 +33416,7 @@
         <v>-10307</v>
       </c>
     </row>
-    <row r="471" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
         <v>2969</v>
       </c>
@@ -33409,7 +33460,7 @@
         <v>6979</v>
       </c>
     </row>
-    <row r="472" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
         <v>2970</v>
       </c>
@@ -33473,7 +33524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <v>2972</v>
       </c>
@@ -33604,7 +33655,7 @@
         <v>7212567</v>
       </c>
     </row>
-    <row r="475" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A475" s="1">
         <v>2973</v>
       </c>
@@ -33735,7 +33786,7 @@
         <v>15896763</v>
       </c>
     </row>
-    <row r="476" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A476" s="1">
         <v>2974</v>
       </c>
@@ -33866,7 +33917,7 @@
         <v>16413487</v>
       </c>
     </row>
-    <row r="477" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A477" s="1">
         <v>2975</v>
       </c>
@@ -33997,7 +34048,7 @@
         <v>7473313</v>
       </c>
     </row>
-    <row r="478" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A478" s="1">
         <v>2976</v>
       </c>
@@ -34128,7 +34179,7 @@
         <v>850159</v>
       </c>
     </row>
-    <row r="479" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A479" s="1">
         <v>2977</v>
       </c>
@@ -34259,7 +34310,7 @@
         <v>9821157</v>
       </c>
     </row>
-    <row r="480" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A480" s="1">
         <v>2978</v>
       </c>
@@ -34390,7 +34441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A481" s="1">
         <v>2979</v>
       </c>
@@ -34521,7 +34572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="482" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A482" s="1">
         <v>2980</v>
       </c>
@@ -34652,7 +34703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A483" s="1">
         <v>2981</v>
       </c>
@@ -34843,7 +34894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A487" s="1">
         <v>2985</v>
       </c>
@@ -34902,7 +34953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="488" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A488" s="1">
         <v>2986</v>
       </c>
@@ -35021,7 +35072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="492" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A492" s="1">
         <v>2990</v>
       </c>
@@ -35065,7 +35116,7 @@
         <v>3664344</v>
       </c>
     </row>
-    <row r="493" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A493" s="1">
         <v>2991</v>
       </c>
@@ -35229,7 +35280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="500" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A500" s="1">
         <v>2998</v>
       </c>
@@ -35288,7 +35339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A501" s="1">
         <v>2999</v>
       </c>
@@ -35348,13 +35399,354 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AQ501" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="FALSE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AQ501" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D245B36-BDFE-4A47-A4CE-E10C3858FCEC}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44545</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5">
+        <v>94633916</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <v>9133015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>815185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
+        <v>85500901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2627142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5">
+        <v>12078731</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1575886</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5">
+        <v>5448558</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5">
+        <v>3113862</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5">
+        <v>611817</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5">
+        <v>16825952</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5">
+        <v>18221796</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5">
+        <v>-436560</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5">
+        <v>6942433</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1895491</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5">
+        <v>513389</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1845457</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="5">
+        <v>392884</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="5">
+        <v>2808702</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="5">
+        <v>3267127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>